<commit_message>
feat: Update HIV_CS for V2.33 translations
</commit_message>
<xml_diff>
--- a/metadata/HIV_CS/HIV_CS_TRACKER_V1_DHIS2.33/reference.xlsx
+++ b/metadata/HIV_CS/HIV_CS_TRACKER_V1_DHIS2.33/reference.xlsx
@@ -506,7 +506,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>HIV_CS_TRACKER_V1.0.0_DHIS2.33_2020-10-10T10:54</v>
+        <v>HIV_CS_TRACKER_V1.0.0_DHIS2.33_2020-10-10T12:37</v>
       </c>
     </row>
   </sheetData>
@@ -791,7 +791,7 @@
         <v>default</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>2020-05-20</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G2" s="4" t="str">
         <v>Bn9otKySZvP</v>
@@ -814,7 +814,7 @@
         <v>default</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>2020-09-29</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G3" s="5" t="str">
         <v>c82CE0oy0Nj</v>
@@ -837,7 +837,7 @@
         <v>default</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>2020-02-10</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G4" s="4" t="str">
         <v>cDt3CvgtlQs</v>
@@ -860,7 +860,7 @@
         <v>default</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>2020-04-03</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G5" s="5" t="str">
         <v>EGjmPoKhHpM</v>
@@ -883,7 +883,7 @@
         <v>default</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>2020-08-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G6" s="4" t="str">
         <v>EZAZ8aIV3kB</v>
@@ -906,7 +906,7 @@
         <v>default</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>2020-08-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G7" s="5" t="str">
         <v>F0GpDqqavuI</v>
@@ -929,7 +929,7 @@
         <v>default</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>2020-08-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G8" s="4" t="str">
         <v>FRRIujn3jHD</v>
@@ -952,7 +952,7 @@
         <v>default</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v>2020-02-10</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G9" s="5" t="str">
         <v>fxXDe8OZ86q</v>
@@ -975,7 +975,7 @@
         <v>default</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>2020-08-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G10" s="4" t="str">
         <v>GCmEFuwLpDN</v>
@@ -998,7 +998,7 @@
         <v>default</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>2020-08-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G11" s="5" t="str">
         <v>HYEdbJEeJbz</v>
@@ -1021,7 +1021,7 @@
         <v>default</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>2020-04-03</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G12" s="4" t="str">
         <v>LGz6njGUAP6</v>
@@ -1044,7 +1044,7 @@
         <v>default</v>
       </c>
       <c r="F13" s="5" t="str">
-        <v>2020-08-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G13" s="5" t="str">
         <v>Lu4jo7fSTb3</v>
@@ -1067,7 +1067,7 @@
         <v>default</v>
       </c>
       <c r="F14" s="4" t="str">
-        <v>2020-04-03</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G14" s="4" t="str">
         <v>Lv3c5VSA9t3</v>
@@ -1090,7 +1090,7 @@
         <v>default</v>
       </c>
       <c r="F15" s="5" t="str">
-        <v>2020-03-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G15" s="5" t="str">
         <v>mUMvkV72WQZ</v>
@@ -1113,7 +1113,7 @@
         <v>default</v>
       </c>
       <c r="F16" s="4" t="str">
-        <v>2020-06-05</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G16" s="4" t="str">
         <v>ncsvQhFKcKc</v>
@@ -1136,7 +1136,7 @@
         <v>default</v>
       </c>
       <c r="F17" s="5" t="str">
-        <v>2020-07-08</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G17" s="5" t="str">
         <v>rcUsYgOnlyF</v>
@@ -1159,7 +1159,7 @@
         <v>default</v>
       </c>
       <c r="F18" s="4" t="str">
-        <v>2020-04-03</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G18" s="4" t="str">
         <v>S4IJiirQVHY</v>
@@ -1182,7 +1182,7 @@
         <v>default</v>
       </c>
       <c r="F19" s="5" t="str">
-        <v>2020-02-11</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G19" s="5" t="str">
         <v>TmAJxu1XNKh</v>
@@ -1205,7 +1205,7 @@
         <v>default</v>
       </c>
       <c r="F20" s="4" t="str">
-        <v>2020-03-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G20" s="4" t="str">
         <v>TQtuEvZ1eF6</v>
@@ -1228,7 +1228,7 @@
         <v>default</v>
       </c>
       <c r="F21" s="5" t="str">
-        <v>2020-02-12</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G21" s="5" t="str">
         <v>uiBCTI2XL2m</v>
@@ -1251,7 +1251,7 @@
         <v>default</v>
       </c>
       <c r="F22" s="4" t="str">
-        <v>2020-03-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G22" s="4" t="str">
         <v>UiX8eZZl3Nt</v>
@@ -1274,7 +1274,7 @@
         <v>default</v>
       </c>
       <c r="F23" s="5" t="str">
-        <v>2020-03-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G23" s="5" t="str">
         <v>v4K5u8wftrq</v>
@@ -1297,7 +1297,7 @@
         <v>default</v>
       </c>
       <c r="F24" s="4" t="str">
-        <v>2020-02-10</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G24" s="4" t="str">
         <v>vAS6qdqF6Gf</v>
@@ -1320,7 +1320,7 @@
         <v>default</v>
       </c>
       <c r="F25" s="5" t="str">
-        <v>2020-02-11</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G25" s="5" t="str">
         <v>VjsXqPWaMNN</v>
@@ -1343,7 +1343,7 @@
         <v>default</v>
       </c>
       <c r="F26" s="4" t="str">
-        <v>2020-02-10</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G26" s="4" t="str">
         <v>zsM4K8kNPSo</v>
@@ -1575,7 +1575,7 @@
         <v>default</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>bjDvmb4bfuf</v>
@@ -1620,7 +1620,7 @@
         <v>default</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-10-08</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>GLevLNI9wkl</v>
@@ -1661,7 +1661,7 @@
         <v>default</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>xYerKDKCefk</v>
@@ -1699,7 +1699,7 @@
         <v>default</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>HllvX50cXC0</v>
@@ -1741,7 +1741,7 @@
         <v>HIV Viral Load Status</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-04-03</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>ADgTXaBsHFi</v>
@@ -1755,7 +1755,7 @@
         <v>TB - IPT Eligibility if negative</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>bH53OxRWzdK</v>
@@ -1769,7 +1769,7 @@
         <v>HIV Modes of Transmission</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-05-15</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>Hr7i8z2nmfW</v>
@@ -1783,7 +1783,7 @@
         <v>HIV ART - Regimens (all)</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2018-05-29</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C5" s="5" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -1797,7 +1797,7 @@
         <v>HIV Follow-up Outcomes</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2020-05-18</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C6" s="4" t="str">
         <v>jkgTCobqE43</v>
@@ -1811,7 +1811,7 @@
         <v>HIV - Sex</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>2020-04-03</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C7" s="5" t="str">
         <v>P0RAq93jsi9</v>
@@ -1825,7 +1825,7 @@
         <v>HIV treatment stopped reasons</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>2020-02-11</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C8" s="4" t="str">
         <v>p4i20eISTFi</v>
@@ -1839,7 +1839,7 @@
         <v>TBT Regimen</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>2020-09-07</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C9" s="5" t="str">
         <v>sE3uCjDohG9</v>
@@ -1853,7 +1853,7 @@
         <v>HIV Follow-up Methods</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>2020-02-10</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C10" s="4" t="str">
         <v>Thh5XshrW4i</v>
@@ -1867,7 +1867,7 @@
         <v>HIV - STATUS</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C11" s="5" t="str">
         <v>Y0L733DyTP2</v>
@@ -1922,7 +1922,7 @@
         <v>DEAD</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>2020-02-11</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E2" s="4" t="str">
         <v>p4i20eISTFi</v>
@@ -1956,7 +1956,7 @@
         <v>4b - AZT-3TC-NVP</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E4" s="4" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -1990,7 +1990,7 @@
         <v>OTHERTPT</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>2020-09-07</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E6" s="4" t="str">
         <v>sE3uCjDohG9</v>
@@ -2007,7 +2007,7 @@
         <v>OTHERUNDETERMINED</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>2020-02-14</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E7" s="5" t="str">
         <v>Hr7i8z2nmfW</v>
@@ -2024,7 +2024,7 @@
         <v>NOTSUPRESSED</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>2020-04-03</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E8" s="4" t="str">
         <v>ADgTXaBsHFi</v>
@@ -2041,7 +2041,7 @@
         <v>1a - TDF-3TC-EFV</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E9" s="5" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2075,7 +2075,7 @@
         <v>NE</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E11" s="5" t="str">
         <v>bH53OxRWzdK</v>
@@ -2092,7 +2092,7 @@
         <v>2b - TDF-3TC-ATVr</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E12" s="4" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2109,7 +2109,7 @@
         <v>2f - ABC+3TC+ATV/r</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E13" s="5" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2126,7 +2126,7 @@
         <v>RESCHEDULED</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v>2020-05-18</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E14" s="4" t="str">
         <v>jkgTCobqE43</v>
@@ -2143,7 +2143,7 @@
         <v>SMS</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v>2020-02-10</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E15" s="5" t="str">
         <v>Thh5XshrW4i</v>
@@ -2160,7 +2160,7 @@
         <v>P</v>
       </c>
       <c r="D16" s="4" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E16" s="4" t="str">
         <v>bH53OxRWzdK</v>
@@ -2177,7 +2177,7 @@
         <v>2a - TDF-3TC-LPVr</v>
       </c>
       <c r="D17" s="5" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E17" s="5" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2194,7 +2194,7 @@
         <v>MOVED</v>
       </c>
       <c r="D18" s="4" t="str">
-        <v>2020-02-11</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E18" s="4" t="str">
         <v>p4i20eISTFi</v>
@@ -2211,7 +2211,7 @@
         <v>1e - AZT-3TC-ABC</v>
       </c>
       <c r="D19" s="5" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E19" s="5" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2228,7 +2228,7 @@
         <v>HOMOSEX</v>
       </c>
       <c r="D20" s="4" t="str">
-        <v>2020-02-14</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E20" s="4" t="str">
         <v>Hr7i8z2nmfW</v>
@@ -2245,7 +2245,7 @@
         <v>1b - AZT-3TC-EFV</v>
       </c>
       <c r="D21" s="5" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E21" s="5" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2279,7 +2279,7 @@
         <v>TG</v>
       </c>
       <c r="D23" s="5" t="str">
-        <v>2020-04-03</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E23" s="5" t="str">
         <v>P0RAq93jsi9</v>
@@ -2296,7 +2296,7 @@
         <v>NOSHOW</v>
       </c>
       <c r="D24" s="4" t="str">
-        <v>2020-02-12</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E24" s="4" t="str">
         <v>p4i20eISTFi</v>
@@ -2313,7 +2313,7 @@
         <v>4d - AZT+3TC+LPV/r</v>
       </c>
       <c r="D25" s="5" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E25" s="5" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2330,7 +2330,7 @@
         <v>TREATMENTSTOPPED</v>
       </c>
       <c r="D26" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E26" s="4" t="str">
         <v>Y0L733DyTP2</v>
@@ -2347,7 +2347,7 @@
         <v>RETAINED</v>
       </c>
       <c r="D27" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E27" s="5" t="str">
         <v>Y0L733DyTP2</v>
@@ -2364,7 +2364,7 @@
         <v>2d - AZT-3TC-ATVr</v>
       </c>
       <c r="D28" s="4" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E28" s="4" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2381,7 +2381,7 @@
         <v>MOTHERTOCHILD</v>
       </c>
       <c r="D29" s="5" t="str">
-        <v>2020-04-03</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E29" s="5" t="str">
         <v>Hr7i8z2nmfW</v>
@@ -2398,7 +2398,7 @@
         <v>TRANSFEROUT</v>
       </c>
       <c r="D30" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E30" s="4" t="str">
         <v>Y0L733DyTP2</v>
@@ -2466,7 +2466,7 @@
         <v>1f - TDF/3TC+NVP</v>
       </c>
       <c r="D34" s="4" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E34" s="4" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2500,7 +2500,7 @@
         <v>CHANGE_STATUS</v>
       </c>
       <c r="D36" s="4" t="str">
-        <v>2020-05-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E36" s="4" t="str">
         <v>jkgTCobqE43</v>
@@ -2517,7 +2517,7 @@
         <v>Commercial_Sex</v>
       </c>
       <c r="D37" s="5" t="str">
-        <v>2020-05-15</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E37" s="5" t="str">
         <v>Hr7i8z2nmfW</v>
@@ -2534,7 +2534,7 @@
         <v>INJECTINGDRUG</v>
       </c>
       <c r="D38" s="4" t="str">
-        <v>2020-02-14</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E38" s="4" t="str">
         <v>Hr7i8z2nmfW</v>
@@ -2551,7 +2551,7 @@
         <v>4a - AZT-3TC-EFV</v>
       </c>
       <c r="D39" s="5" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E39" s="5" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2568,7 +2568,7 @@
         <v>NNE</v>
       </c>
       <c r="D40" s="4" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E40" s="4" t="str">
         <v>bH53OxRWzdK</v>
@@ -2602,7 +2602,7 @@
         <v>2e - ABC+3TC+LPV/r</v>
       </c>
       <c r="D42" s="4" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E42" s="4" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2619,7 +2619,7 @@
         <v>2c - AZT-3TC-LPVr</v>
       </c>
       <c r="D43" s="5" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E43" s="5" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2636,7 +2636,7 @@
         <v>NORESPONSE</v>
       </c>
       <c r="D44" s="4" t="str">
-        <v>2020-05-18</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E44" s="4" t="str">
         <v>jkgTCobqE43</v>
@@ -2653,7 +2653,7 @@
         <v>SUPRESSED</v>
       </c>
       <c r="D45" s="5" t="str">
-        <v>2020-04-03</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E45" s="5" t="str">
         <v>ADgTXaBsHFi</v>
@@ -2670,7 +2670,7 @@
         <v>1d - ABC+3TC+EFV</v>
       </c>
       <c r="D46" s="4" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E46" s="4" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2687,7 +2687,7 @@
         <v>HETEROSEXUAL</v>
       </c>
       <c r="D47" s="5" t="str">
-        <v>2020-05-15</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E47" s="5" t="str">
         <v>Hr7i8z2nmfW</v>
@@ -2721,7 +2721,7 @@
         <v>PhoneCall</v>
       </c>
       <c r="D49" s="5" t="str">
-        <v>2020-02-10</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E49" s="5" t="str">
         <v>Thh5XshrW4i</v>
@@ -2738,7 +2738,7 @@
         <v>HOMEVISIT</v>
       </c>
       <c r="D50" s="4" t="str">
-        <v>2020-02-10</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E50" s="4" t="str">
         <v>Thh5XshrW4i</v>
@@ -2755,7 +2755,7 @@
         <v>4d - TDF+3TC+EFV</v>
       </c>
       <c r="D51" s="5" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E51" s="5" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2789,7 +2789,7 @@
         <v>1g - Others</v>
       </c>
       <c r="D53" s="5" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E53" s="5" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2823,7 +2823,7 @@
         <v>Scheduled</v>
       </c>
       <c r="D55" s="5" t="str">
-        <v>2020-05-18</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E55" s="5" t="str">
         <v>jkgTCobqE43</v>
@@ -2840,7 +2840,7 @@
         <v>1c - AZT-3TC-NVP</v>
       </c>
       <c r="D56" s="4" t="str">
-        <v>2018-05-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E56" s="4" t="str">
         <v>i1ZlYkC3v1Z</v>
@@ -2991,7 +2991,7 @@
         <v>Percentage</v>
       </c>
       <c r="I4" s="4" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="J4" s="4" t="str">
         <v/>
@@ -3023,7 +3023,7 @@
         <v>Percentage</v>
       </c>
       <c r="I5" s="5" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="J5" s="5" t="str">
         <v/>
@@ -3087,7 +3087,7 @@
         <v>Percentage</v>
       </c>
       <c r="I7" s="5" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="J7" s="5" t="str">
         <v/>
@@ -3119,7 +3119,7 @@
         <v>Percentage</v>
       </c>
       <c r="I8" s="4" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="J8" s="4" t="str">
         <v/>
@@ -3215,7 +3215,7 @@
         <v>Percentage</v>
       </c>
       <c r="I11" s="5" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="J11" s="5" t="str">
         <v/>
@@ -3285,7 +3285,7 @@
         <v>Person</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-08-13</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>MCPQUTHX1Ze</v>
@@ -3375,7 +3375,7 @@
         <v/>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-06-17</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>KKvBWmeIsvN</v>
@@ -3389,7 +3389,7 @@
         <v/>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2020-06-17</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>s7DBTTX68Lk</v>
@@ -3990,7 +3990,7 @@
         <v>HIV CS 5. - TB Preventive Treatment</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-09-18</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>hltk73PwPCr</v>
@@ -4012,7 +4012,7 @@
         <v>HIV CS 4. - Viral Load</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-09-18</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>Uy1cjNuoJcJ</v>
@@ -4023,7 +4023,7 @@
         <v>HIV CS - 2. Case Reporting &amp; Demographics</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2020-10-09</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C5" s="5" t="str">
         <v>vHJr37SQiie</v>
@@ -4034,7 +4034,7 @@
         <v>HIV CS 3. - ART Linkage &amp; Retention</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2020-10-01</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C6" s="4" t="str">
         <v>wvMQ7MWdBiZ</v>
@@ -5578,7 +5578,7 @@
         <v>Includes all enrollments since last analytics run; excludes enrollments marked "DEAD" or "TRANSFER OUT"; User OU</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-10-01</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>B45PDFcbuHs</v>
@@ -5592,7 +5592,7 @@
         <v>Excludes enrollments marked "DEAD" or "TRANSFERRED"</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2020-10-09</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>ChiW0QCYsoQ</v>
@@ -5606,7 +5606,7 @@
         <v>By positive test month</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D4" s="4" t="str">
         <v>F8jbT7QbQOi</v>
@@ -5704,7 +5704,7 @@
         <v xml:space="preserve">Persons living with HIV who have been initiated on ART within 14 days or enrollment in the programme. </v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D11" s="5" t="str">
         <v>JxQki1vvSq6</v>
@@ -5718,7 +5718,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D12" s="4" t="str">
         <v>Jz5QANzFZnp</v>
@@ -5732,7 +5732,7 @@
         <v>Excludes enrollments marked "DEAD" or "TRANSFERRED"</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>2020-10-09</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D13" s="5" t="str">
         <v>k1UByb9qmse</v>
@@ -5746,7 +5746,7 @@
         <v>Includes all enrollments since last analytics run; excludes enrollments marked "DEAD" or "LOST TO FOLLOW UP", user OU</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>2020-10-01</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D14" s="4" t="str">
         <v>M7vkuYqrZNI</v>
@@ -5788,7 +5788,7 @@
         <v>Includes all enrollments since last analytics run; excludes enrollments marked "DEAD" or "TRANSFER OUT"; User OU</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>2020-10-01</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D17" s="5" t="str">
         <v>nIj1eWinEZw</v>
@@ -5816,7 +5816,7 @@
         <v>Just new by month; excludes enrollments marked "DEAD" or "TRANSFER OUT"; User OU</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>2020-06-15</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D19" s="5" t="str">
         <v>p2g3v3VoBRF</v>
@@ -5844,7 +5844,7 @@
         <v>Just new by month; excludes enrollments marked "DEAD" or "TRANSFER OUT"; User OU</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>2020-09-17</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D21" s="5" t="str">
         <v>PRHBnRA0nCZ</v>
@@ -5858,7 +5858,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D22" s="4" t="str">
         <v>ps2h9StSxb3</v>
@@ -5886,7 +5886,7 @@
         <v>Excludes enrollments marked "DEAD" or "TRANSFERRED"</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>2020-10-09</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D24" s="4" t="str">
         <v>rIUI6cWrFDY</v>
@@ -5900,7 +5900,7 @@
         <v>Includes all enrollments since last analytics run; excludes enrollments marked "DEAD" or "LOST TO FOLLOW UP", user OU</v>
       </c>
       <c r="C25" s="5" t="str">
-        <v>2020-10-01</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D25" s="5" t="str">
         <v>RmoFauv1u9d</v>
@@ -5928,7 +5928,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C27" s="5" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D27" s="5" t="str">
         <v>VR7NwguSGU9</v>
@@ -5984,7 +5984,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C31" s="5" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D31" s="5" t="str">
         <v>ZmxEOhZP9UJ</v>
@@ -6057,7 +6057,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D4" s="4" t="str">
         <v>JmAddDaVNs2</v>
@@ -6085,7 +6085,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D6" s="4" t="str">
         <v>QgzrubS8YKo</v>
@@ -6113,7 +6113,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2020-06-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D8" s="4" t="str">
         <v>tU9RH0c3Wyq</v>
@@ -6127,7 +6127,7 @@
         <v>Total to date</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2020-10-09</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D9" s="5" t="str">
         <v>w2d0XT59gqd</v>
@@ -6217,7 +6217,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-06-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>hHmP3wjdqiv</v>
@@ -6231,7 +6231,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>S5WE5dc0hiZ</v>
@@ -6245,7 +6245,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2020-10-01</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D4" s="4" t="str">
         <v>VztTOyOsrUR</v>
@@ -6304,7 +6304,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>Brw5CeNlGbk</v>
@@ -6318,7 +6318,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2020-06-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>FrdwzlGYC4r</v>
@@ -6425,7 +6425,7 @@
         <v>HIV Indicator Descriptions: Overall</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-06-15</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>TEi83i86buD</v>
@@ -6463,7 +6463,7 @@
         <v>HIV Case Surveillance</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-09-28</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>pm1eqD1fqwx</v>
@@ -6553,7 +6553,7 @@
         <v>Family name of the patient</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>2020-08-13</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E2" s="4" t="str">
         <v>aW66s2QSosT</v>
@@ -6570,7 +6570,7 @@
         <v/>
       </c>
       <c r="D3" s="5" t="str">
-        <v>2020-08-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E3" s="5" t="str">
         <v>ciCR6BBvIT4</v>
@@ -6604,7 +6604,7 @@
         <v>HIV Program ID (For example, ART Number)</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>2020-07-08</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E5" s="5" t="str">
         <v>iZWtxl8sCi6</v>
@@ -6621,7 +6621,7 @@
         <v/>
       </c>
       <c r="D6" s="4" t="str">
-        <v>2020-09-29</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E6" s="4" t="str">
         <v>Jt68iauILtD</v>
@@ -6638,7 +6638,7 @@
         <v>Date of birth plus calculated age</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E7" s="5" t="str">
         <v>mAWcalQYYyk</v>
@@ -6655,7 +6655,7 @@
         <v>From master facility list</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>2020-08-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E8" s="4" t="str">
         <v>sWn0CERcUYj</v>
@@ -6672,7 +6672,7 @@
         <v>The name of the patient or initials</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>2020-08-13</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E9" s="5" t="str">
         <v>TfdH5KvFmMy</v>
@@ -6689,7 +6689,7 @@
         <v xml:space="preserve">The National Health Information System ID </v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>2020-08-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E10" s="4" t="str">
         <v>u101Hz0Lemb</v>
@@ -6706,7 +6706,7 @@
         <v>Current home address of the patient</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E11" s="5" t="str">
         <v>VCtm2pySeEV</v>
@@ -6723,7 +6723,7 @@
         <v/>
       </c>
       <c r="D12" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E12" s="4" t="str">
         <v>Z1rLc1rVHK8</v>
@@ -6768,7 +6768,7 @@
         <v>Person</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-09-15</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -6813,7 +6813,7 @@
         <v>ang4CLldbIu</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-09-28T21:13:49.585</v>
+        <v>2020-10-10T12:21:56.463</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -6827,7 +6827,7 @@
         <v>K5ac7u3V5bB</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2020-09-28T21:13:49.583</v>
+        <v>2020-10-10T12:21:56.299</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -6841,7 +6841,7 @@
         <v>UvYb6qJpQu0</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2020-09-28T21:13:49.588</v>
+        <v>2020-10-10T12:21:56.148</v>
       </c>
       <c r="D4" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -7194,7 +7194,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G2" s="4" t="str">
-        <v>2020-06-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H2" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -7220,7 +7220,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G3" s="5" t="str">
-        <v>2020-05-20</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H3" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7246,7 +7246,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G4" s="4" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H4" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -7272,7 +7272,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G5" s="5" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H5" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7298,7 +7298,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G6" s="4" t="str">
-        <v>2020-06-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H6" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -7324,7 +7324,7 @@
         <v>EVENT</v>
       </c>
       <c r="G7" s="5" t="str">
-        <v>2020-05-20</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H7" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7350,7 +7350,7 @@
         <v>EVENT</v>
       </c>
       <c r="G8" s="4" t="str">
-        <v>2020-05-20</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H8" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -7376,7 +7376,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G9" s="5" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H9" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7402,7 +7402,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G10" s="4" t="str">
-        <v>2020-05-20</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H10" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -7428,7 +7428,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G11" s="5" t="str">
-        <v>2020-06-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H11" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7454,7 +7454,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G12" s="4" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H12" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -7480,7 +7480,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G13" s="5" t="str">
-        <v>2020-06-15</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H13" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7532,7 +7532,7 @@
         <v>EVENT</v>
       </c>
       <c r="G15" s="5" t="str">
-        <v>2020-05-20</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H15" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7558,7 +7558,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G16" s="4" t="str">
-        <v>2020-10-09</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H16" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -7584,7 +7584,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G17" s="5" t="str">
-        <v>2020-06-15</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H17" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7610,7 +7610,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G18" s="4" t="str">
-        <v>2020-09-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H18" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -7636,7 +7636,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G19" s="5" t="str">
-        <v>2020-06-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H19" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7662,7 +7662,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G20" s="4" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H20" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -7688,7 +7688,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G21" s="5" t="str">
-        <v>2020-06-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H21" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7714,7 +7714,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G22" s="4" t="str">
-        <v>2020-06-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H22" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -7740,7 +7740,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G23" s="5" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H23" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7766,7 +7766,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G24" s="4" t="str">
-        <v>2020-06-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H24" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -7792,7 +7792,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G25" s="5" t="str">
-        <v>2020-06-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H25" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7844,7 +7844,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G27" s="5" t="str">
-        <v>2020-05-20</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H27" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7870,7 +7870,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G28" s="4" t="str">
-        <v>2020-06-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H28" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -7896,7 +7896,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G29" s="5" t="str">
-        <v>2020-06-15</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H29" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7922,7 +7922,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G30" s="4" t="str">
-        <v>2020-05-20</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H30" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -7948,7 +7948,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G31" s="5" t="str">
-        <v>2020-06-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H31" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -7974,7 +7974,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G32" s="4" t="str">
-        <v>2020-06-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H32" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8000,7 +8000,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G33" s="5" t="str">
-        <v>2020-06-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H33" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8026,7 +8026,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G34" s="4" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H34" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8078,7 +8078,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G36" s="4" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H36" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8104,7 +8104,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G37" s="5" t="str">
-        <v>2020-06-15</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H37" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8130,7 +8130,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G38" s="4" t="str">
-        <v>2020-06-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H38" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8156,7 +8156,7 @@
         <v>EVENT</v>
       </c>
       <c r="G39" s="5" t="str">
-        <v>2020-05-20</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H39" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8182,7 +8182,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G40" s="4" t="str">
-        <v>2020-06-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H40" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8208,7 +8208,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G41" s="5" t="str">
-        <v>2020-06-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H41" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8234,7 +8234,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G42" s="4" t="str">
-        <v>2020-06-15</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H42" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8260,7 +8260,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G43" s="5" t="str">
-        <v>2020-05-20</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H43" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8286,7 +8286,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G44" s="4" t="str">
-        <v>2020-06-25</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H44" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8312,7 +8312,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G45" s="5" t="str">
-        <v>2020-06-19</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H45" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8338,7 +8338,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G46" s="4" t="str">
-        <v>2020-07-03</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H46" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8390,7 +8390,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G48" s="4" t="str">
-        <v>2020-07-03</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H48" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8442,7 +8442,7 @@
         <v/>
       </c>
       <c r="D2" s="4" t="str">
-        <v>2020-05-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E2" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8459,7 +8459,7 @@
         <v/>
       </c>
       <c r="D3" s="5" t="str">
-        <v>2020-05-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E3" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8476,7 +8476,7 @@
         <v>Date of current Event PLUS amount of days with Medicine</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>2020-09-07</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E4" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8493,7 +8493,7 @@
         <v>Displays the date a treatment was completed it if was previously completed.</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>2020-09-28</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E5" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8510,7 +8510,7 @@
         <v/>
       </c>
       <c r="D6" s="4" t="str">
-        <v>2020-05-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E6" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8527,7 +8527,7 @@
         <v/>
       </c>
       <c r="D7" s="5" t="str">
-        <v>2020-10-01</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E7" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8544,7 +8544,7 @@
         <v>The HIV test cannot be before the patient was born</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>2020-02-11</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E8" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8561,7 +8561,7 @@
         <v/>
       </c>
       <c r="D9" s="5" t="str">
-        <v>2020-10-01</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E9" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8578,7 +8578,7 @@
         <v>If the days between the date of initiation or previous date of initiation are less than 180, then hide Viral load status</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>2020-09-28</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E10" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8612,7 +8612,7 @@
         <v>Hide treatment section if treatment not started</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>2020-10-01</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E12" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8629,7 +8629,7 @@
         <v>if a phone number was entered, it shows it.</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E13" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8646,7 +8646,7 @@
         <v>Displays if previously eligible for TPT</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v>2020-05-20</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E14" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8663,7 +8663,7 @@
         <v>If the days between the date of initiation or previous date of initiation are less than 180, then show message "Viral load tests should only be performed after six months on treatment"</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v>2020-09-28</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E15" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8680,7 +8680,7 @@
         <v/>
       </c>
       <c r="D16" s="4" t="str">
-        <v>2020-02-11</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E16" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8697,7 +8697,7 @@
         <v>Displays the date a treatment was initiated it if was previously initiated</v>
       </c>
       <c r="D17" s="5" t="str">
-        <v>2020-05-20</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E17" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8714,7 +8714,7 @@
         <v/>
       </c>
       <c r="D18" s="4" t="str">
-        <v>2020-02-17</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E18" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8731,7 +8731,7 @@
         <v/>
       </c>
       <c r="D19" s="5" t="str">
-        <v>2020-05-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E19" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8748,7 +8748,7 @@
         <v/>
       </c>
       <c r="D20" s="4" t="str">
-        <v>2020-10-01</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E20" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8765,7 +8765,7 @@
         <v>Displays the TPT regimen the patient is following</v>
       </c>
       <c r="D21" s="5" t="str">
-        <v>2020-09-29</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E21" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8782,7 +8782,7 @@
         <v>Hide Viral load test results if viral load is under 1000</v>
       </c>
       <c r="D22" s="4" t="str">
-        <v>2020-04-06</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E22" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8816,7 +8816,7 @@
         <v xml:space="preserve">THis is so that we have a constant date for when the treatment was initiated and we can calculate indicators. </v>
       </c>
       <c r="D24" s="4" t="str">
-        <v>2020-03-31</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E24" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8833,7 +8833,7 @@
         <v/>
       </c>
       <c r="D25" s="5" t="str">
-        <v>2020-07-08</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E25" s="5" t="str">
         <v>Xh88p1nyefp</v>
@@ -8850,7 +8850,7 @@
         <v>Displays the date a patient became eligible for TPT from the first time they became eligible.</v>
       </c>
       <c r="D26" s="4" t="str">
-        <v>2020-08-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E26" s="4" t="str">
         <v>Xh88p1nyefp</v>
@@ -8867,7 +8867,7 @@
         <v>If a patient has not had medicine for more than 28 days, then they are lost to follow-up. It counts days since last visit and current date</v>
       </c>
       <c r="D27" s="5" t="str">
-        <v>2020-10-01</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E27" s="5" t="str">
         <v>Xh88p1nyefp</v>

</xml_diff>